<commit_message>
S10004, S10005, S10006, S10007
</commit_message>
<xml_diff>
--- a/tl/S10004.MES.BIN.xlsx
+++ b/tl/S10004.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49522FF3-57AE-40C9-A119-166CC39714A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910A0082-B63B-4535-8806-3FEC9E0DB2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="8745" windowWidth="53205" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="8190" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S10004.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>